<commit_message>
Assertion & Excel Write
</commit_message>
<xml_diff>
--- a/InputData.xlsx
+++ b/InputData.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="15">
   <si>
     <t>Meet</t>
   </si>
@@ -1227,85 +1227,172 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleSheetLayoutView="60" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.2857142857143" defaultRowHeight="15" outlineLevelRow="4" outlineLevelCol="2"/>
   <cols>
-    <col min="2" max="2" width="18.1428571428571" customWidth="1"/>
-    <col min="3" max="3" width="12.8571428571429" customWidth="1"/>
+    <col min="2" max="2" customWidth="true" width="19.4285714285714"/>
+    <col min="3" max="3" customWidth="true" width="12.8571428571429"/>
+    <col min="5" max="5" customWidth="true" width="18.0"/>
+    <col min="6" max="6" customWidth="true" width="13.7142857142857"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" t="s">
+      <c r="A1" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s" s="0">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" t="s" s="0">
+        <v>0</v>
+      </c>
+      <c r="E1" t="s" s="0">
+        <v>1</v>
+      </c>
+      <c r="F1" t="s" s="0">
+        <v>2</v>
+      </c>
+      <c r="G1" t="s" s="0">
+        <v>0</v>
+      </c>
+      <c r="H1" t="s" s="0">
+        <v>1</v>
+      </c>
+      <c r="I1" t="s" s="0">
+        <v>2</v>
+      </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" t="s">
+      <c r="A2" t="s" s="0">
         <v>3</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" t="s" s="0">
         <v>4</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="D2" t="s" s="0">
+        <v>3</v>
+      </c>
+      <c r="E2" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="F2" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="G2" t="s" s="0">
+        <v>3</v>
+      </c>
+      <c r="H2" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="I2" t="s" s="0">
+        <v>5</v>
+      </c>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" t="s">
+      <c r="A3" t="s" s="0">
         <v>6</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" t="s" s="0">
         <v>7</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="D3" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="E3" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="F3" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="G3" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="H3" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="I3" t="s" s="0">
+        <v>8</v>
+      </c>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4" t="s">
+      <c r="A4" t="s" s="0">
         <v>9</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" t="s" s="0">
         <v>10</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>11</v>
       </c>
+      <c r="D4" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="E4" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="F4" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="G4" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="H4" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="I4" t="s" s="0">
+        <v>11</v>
+      </c>
     </row>
     <row r="5" spans="1:3">
-      <c r="A5" t="s">
+      <c r="A5" t="s" s="0">
         <v>12</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" t="s" s="0">
         <v>13</v>
       </c>
       <c r="C5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="E5" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="F5" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="G5" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="H5" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="I5" t="s" s="0">
         <v>14</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B1" r:id="rId1" display="meet@gmail.com"/>
-    <hyperlink ref="B2" r:id="rId2" display="meet1@gmail.com" tooltip="mailto:meet1@gmail.com"/>
-    <hyperlink ref="B3" r:id="rId3" display="meet2@gmail.com" tooltip="mailto:meet2@gmail.com"/>
-    <hyperlink ref="B4" r:id="rId4" display="meet3@gmail.com" tooltip="mailto:meet3@gmail.com"/>
-    <hyperlink ref="B5" r:id="rId5" display="meet4@gmail.com" tooltip="mailto:meet4@gmail.com"/>
-    <hyperlink ref="C1" r:id="rId6" display="Meet@123"/>
-    <hyperlink ref="C2" r:id="rId7" display="Meet2@124" tooltip="mailto:Meet2@124"/>
-    <hyperlink ref="C3" r:id="rId8" display="Meet3@125" tooltip="mailto:Meet3@125"/>
-    <hyperlink ref="C4" r:id="rId9" display="Meet4@126" tooltip="mailto:Meet4@126"/>
-    <hyperlink ref="C5" r:id="rId10" display="Meet5@127" tooltip="mailto:Meet5@127"/>
+    <hyperlink ref="C1" r:id="rId1" display="Meet@123"/>
+    <hyperlink ref="C2" r:id="rId2" display="Meet2@124" tooltip="mailto:Meet2@124"/>
+    <hyperlink ref="C3" r:id="rId3" display="Meet3@125" tooltip="mailto:Meet3@125"/>
+    <hyperlink ref="C4" r:id="rId4" display="Meet4@126" tooltip="mailto:Meet4@126"/>
+    <hyperlink ref="C5" r:id="rId5" display="Meet5@127" tooltip="mailto:Meet5@127"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>